<commit_message>
pictureBox focus steal fix
</commit_message>
<xml_diff>
--- a/Publication/ClipboardManagerComparison.xlsx
+++ b/Publication/ClipboardManagerComparison.xlsx
@@ -46,9 +46,6 @@
   </si>
   <si>
     <t>ClipDiary</t>
-  </si>
-  <si>
-    <t>Used defined clip categories</t>
   </si>
   <si>
     <t>Multipaste as plain text</t>
@@ -367,6 +364,9 @@
   </si>
   <si>
     <t>Просмотр Rich text клипов с родным оформлением</t>
+  </si>
+  <si>
+    <t>User defined clip categories</t>
   </si>
 </sst>
 </file>
@@ -783,8 +783,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G41"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H1" sqref="H1"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="B44" sqref="B44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -797,7 +797,7 @@
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B1" s="4" t="s">
         <v>0</v>
@@ -815,915 +815,915 @@
         <v>9</v>
       </c>
       <c r="G1" s="6" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="2" spans="1:7">
       <c r="A2" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D2" s="8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E2" s="8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F2" s="7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G2" s="7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="3" spans="1:7">
       <c r="A3" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D3" s="7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E3" s="8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F3" s="7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G3" s="7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="4" spans="1:7">
       <c r="A4" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E4" s="8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F4" s="8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G4" s="8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="5" spans="1:7">
       <c r="A5" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D5" s="8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E5" s="8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F5" s="7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G5" s="7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="6" spans="1:7">
       <c r="A6" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C6" s="8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D6" s="7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E6" s="7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F6" s="8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G6" s="8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="7" spans="1:7">
       <c r="A7" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B7" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="B7" s="1" t="s">
-        <v>57</v>
-      </c>
       <c r="C7" s="8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D7" s="7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E7" s="7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F7" s="7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G7" s="8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="8" spans="1:7">
       <c r="A8" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D8" s="8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E8" s="8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F8" s="7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G8" s="7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="9" spans="1:7">
       <c r="A9" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D9" s="7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E9" s="8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F9" s="7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G9" s="7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="10" spans="1:7">
       <c r="A10" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C10" s="8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D10" s="7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E10" s="7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F10" s="8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G10" s="8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="11" spans="1:7">
       <c r="A11" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C11" s="8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D11" s="7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E11" s="8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F11" s="7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G11" s="7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="12" spans="1:7">
       <c r="A12" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C12" s="8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D12" s="8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E12" s="7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F12" s="7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G12" s="7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="13" spans="1:7">
       <c r="A13" s="3" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C13" s="8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D13" s="8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E13" s="8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F13" s="8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G13" s="7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="14" spans="1:7">
       <c r="A14" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C14" s="8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D14" s="8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E14" s="8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F14" s="7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G14" s="8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="15" spans="1:7">
       <c r="A15" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C15" s="8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D15" s="7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E15" s="7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F15" s="7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G15" s="7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="16" spans="1:7">
       <c r="A16" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C16" s="8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D16" s="7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E16" s="8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F16" s="7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G16" s="7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="17" spans="1:7">
       <c r="A17" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B17" s="9" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C17" s="8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D17" s="7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E17" s="7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F17" s="8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G17" s="8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="18" spans="1:7">
       <c r="A18" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C18" s="8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D18" s="7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E18" s="7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F18" s="8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G18" s="7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="19" spans="1:7">
       <c r="A19" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C19" s="8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D19" s="8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E19" s="7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F19" s="7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G19" s="7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="20" spans="1:7">
       <c r="A20" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C20" s="8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D20" s="7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E20" s="7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F20" s="7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G20" s="8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="21" spans="1:7">
       <c r="A21" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B21" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="B21" s="1" t="s">
-        <v>53</v>
-      </c>
       <c r="C21" s="8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D21" s="7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E21" s="7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F21" s="7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G21" s="7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="22" spans="1:7">
       <c r="A22" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C22" s="8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D22" s="7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E22" s="8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F22" s="7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G22" s="8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="23" spans="1:7">
       <c r="A23" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C23" s="8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D23" s="7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E23" s="8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F23" s="8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G23" s="7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="24" spans="1:7">
       <c r="A24" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C24" s="8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D24" s="7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E24" s="7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F24" s="7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G24" s="7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="25" spans="1:7">
       <c r="A25" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C25" s="8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D25" s="7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E25" s="7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F25" s="8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G25" s="7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="26" spans="1:7">
       <c r="A26" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C26" s="8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D26" s="8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E26" s="8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F26" s="7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G26" s="7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="27" spans="1:7">
       <c r="A27" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="B27" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="B27" s="3" t="s">
-        <v>73</v>
-      </c>
       <c r="C27" s="8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D27" s="8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E27" s="8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F27" s="7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G27" s="7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="28" spans="1:7">
       <c r="A28" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C28" s="8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D28" s="8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E28" s="8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F28" s="7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G28" s="7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="29" spans="1:7">
       <c r="A29" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B29" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C29" s="8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D29" s="7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E29" s="7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F29" s="7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G29" s="7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="30" spans="1:7">
       <c r="A30" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C30" s="8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D30" s="7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E30" s="7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F30" s="8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G30" s="8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="31" spans="1:7">
       <c r="A31" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B31" s="1" t="s">
         <v>3</v>
       </c>
       <c r="C31" s="8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D31" s="7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E31" s="7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F31" s="8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G31" s="8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="32" spans="1:7">
       <c r="A32" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B32" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C32" s="8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D32" s="7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E32" s="8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F32" s="7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G32" s="7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="33" spans="1:7">
       <c r="A33" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B33" s="1" t="s">
         <v>2</v>
       </c>
       <c r="C33" s="8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D33" s="7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E33" s="8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F33" s="8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G33" s="8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="34" spans="1:7">
       <c r="A34" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B34" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C34" s="8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D34" s="8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E34" s="8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F34" s="7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G34" s="7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="35" spans="1:7">
       <c r="A35" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C35" s="8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D35" s="7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E35" s="8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F35" s="7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G35" s="8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="36" spans="1:7">
       <c r="A36" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C36" s="8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D36" s="7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E36" s="7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F36" s="7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G36" s="8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="37" spans="1:7">
       <c r="A37" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C37" s="7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D37" s="7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E37" s="8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F37" s="7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G37" s="7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="38" spans="1:7">
       <c r="A38" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C38" s="8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D38" s="8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E38" s="8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F38" s="7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G38" s="7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="39" spans="1:7">
       <c r="A39" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C39" s="8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D39" s="8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E39" s="8" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F39" s="8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G39" s="8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="40" spans="1:7">
       <c r="A40" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>10</v>
+        <v>91</v>
       </c>
       <c r="C40" s="7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D40" s="8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E40" s="8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F40" s="8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G40" s="7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="41" spans="1:7">
       <c r="A41" s="3" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B41" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C41" s="7" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D41" s="8">
         <v>30</v>
@@ -1735,7 +1735,7 @@
         <v>30</v>
       </c>
       <c r="G41" s="8" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
+commands "add/set text in filter" + rtf, html type filters
</commit_message>
<xml_diff>
--- a/Publication/ClipboardManagerComparison.xlsx
+++ b/Publication/ClipboardManagerComparison.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="284" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="289" uniqueCount="97">
   <si>
     <t>Feature</t>
   </si>
@@ -367,6 +367,21 @@
   </si>
   <si>
     <t>70</t>
+  </si>
+  <si>
+    <t>1.35</t>
+  </si>
+  <si>
+    <t>3.21</t>
+  </si>
+  <si>
+    <t>5.1</t>
+  </si>
+  <si>
+    <t>3.1.6</t>
+  </si>
+  <si>
+    <t>5.23</t>
   </si>
 </sst>
 </file>
@@ -781,10 +796,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G41"/>
+  <dimension ref="A1:G42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="C42" sqref="C42"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -819,58 +834,54 @@
       </c>
     </row>
     <row r="2" spans="1:7">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="4"/>
+      <c r="B2" s="4"/>
+      <c r="C2" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>96</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>93</v>
+      </c>
+      <c r="F2" s="6" t="s">
+        <v>94</v>
+      </c>
+      <c r="G2" s="6" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
+      <c r="A3" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B3" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="C2" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="D2" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="E2" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="F2" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="G2" s="7" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7">
-      <c r="A3" s="3" t="s">
+      <c r="C3" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="D3" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="E3" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="F3" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="G3" s="7" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
+      <c r="A4" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B4" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="C3" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="D3" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="E3" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="F3" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="G3" s="7" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7">
-      <c r="A4" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>34</v>
-      </c>
       <c r="C4" s="8" t="s">
         <v>30</v>
       </c>
@@ -880,65 +891,65 @@
       <c r="E4" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="F4" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="G4" s="8" t="s">
-        <v>30</v>
+      <c r="F4" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="G4" s="7" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="5" spans="1:7">
       <c r="A5" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C5" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="D5" s="8" t="s">
-        <v>30</v>
+        <v>34</v>
+      </c>
+      <c r="C5" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="D5" s="7" t="s">
+        <v>29</v>
       </c>
       <c r="E5" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="F5" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="G5" s="7" t="s">
-        <v>29</v>
+      <c r="F5" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="G5" s="8" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="6" spans="1:7">
       <c r="A6" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="C6" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="D6" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="E6" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="F6" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="G6" s="8" t="s">
-        <v>30</v>
+        <v>14</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="D6" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="E6" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="F6" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="G6" s="7" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="7" spans="1:7">
       <c r="A7" s="1" t="s">
-        <v>53</v>
+        <v>37</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>54</v>
+        <v>20</v>
       </c>
       <c r="C7" s="8" t="s">
         <v>30</v>
@@ -949,8 +960,8 @@
       <c r="E7" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="F7" s="7" t="s">
-        <v>29</v>
+      <c r="F7" s="8" t="s">
+        <v>30</v>
       </c>
       <c r="G7" s="8" t="s">
         <v>30</v>
@@ -958,45 +969,45 @@
     </row>
     <row r="8" spans="1:7">
       <c r="A8" s="1" t="s">
-        <v>38</v>
+        <v>53</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C8" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="D8" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="E8" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="F8" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="G8" s="7" t="s">
-        <v>29</v>
+        <v>54</v>
+      </c>
+      <c r="C8" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="D8" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="E8" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="F8" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="G8" s="8" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="9" spans="1:7">
       <c r="A9" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C9" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="D9" s="7" t="s">
-        <v>29</v>
+      <c r="D9" s="8" t="s">
+        <v>30</v>
       </c>
       <c r="E9" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="F9" s="7" t="s">
-        <v>29</v>
+      <c r="F9" s="8" t="s">
+        <v>31</v>
       </c>
       <c r="G9" s="7" t="s">
         <v>29</v>
@@ -1004,33 +1015,33 @@
     </row>
     <row r="10" spans="1:7">
       <c r="A10" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="C10" s="8" t="s">
-        <v>30</v>
+        <v>15</v>
+      </c>
+      <c r="C10" s="7" t="s">
+        <v>29</v>
       </c>
       <c r="D10" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="E10" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="F10" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="G10" s="8" t="s">
-        <v>30</v>
+      <c r="E10" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="F10" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="G10" s="7" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="11" spans="1:7">
       <c r="A11" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>41</v>
+        <v>26</v>
       </c>
       <c r="C11" s="8" t="s">
         <v>30</v>
@@ -1038,69 +1049,69 @@
       <c r="D11" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="E11" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="F11" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="G11" s="7" t="s">
-        <v>29</v>
+      <c r="E11" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="F11" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="G11" s="8" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="12" spans="1:7">
       <c r="A12" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C12" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="D12" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="E12" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="F12" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="G12" s="7" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7">
+      <c r="A13" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="B12" s="1" t="s">
+      <c r="B13" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="C12" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="D12" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="E12" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="F12" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="G12" s="7" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7">
-      <c r="A13" s="3" t="s">
+      <c r="C13" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="D13" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="E13" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="F13" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="G13" s="7" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7">
+      <c r="A14" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="B13" s="3" t="s">
+      <c r="B14" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="C13" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="D13" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="E13" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="F13" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="G13" s="7" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7">
-      <c r="A14" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>44</v>
-      </c>
       <c r="C14" s="8" t="s">
         <v>30</v>
       </c>
@@ -1110,42 +1121,42 @@
       <c r="E14" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="F14" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="G14" s="8" t="s">
-        <v>30</v>
+      <c r="F14" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="G14" s="7" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="15" spans="1:7">
       <c r="A15" s="1" t="s">
-        <v>80</v>
+        <v>45</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>79</v>
+        <v>44</v>
       </c>
       <c r="C15" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="D15" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="E15" s="7" t="s">
-        <v>29</v>
+      <c r="D15" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="E15" s="8" t="s">
+        <v>30</v>
       </c>
       <c r="F15" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="G15" s="7" t="s">
-        <v>29</v>
+      <c r="G15" s="8" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="16" spans="1:7">
       <c r="A16" s="1" t="s">
-        <v>46</v>
+        <v>80</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>12</v>
+        <v>79</v>
       </c>
       <c r="C16" s="8" t="s">
         <v>30</v>
@@ -1153,8 +1164,8 @@
       <c r="D16" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="E16" s="8" t="s">
-        <v>30</v>
+      <c r="E16" s="7" t="s">
+        <v>29</v>
       </c>
       <c r="F16" s="7" t="s">
         <v>29</v>
@@ -1165,10 +1176,10 @@
     </row>
     <row r="17" spans="1:7">
       <c r="A17" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="B17" s="9" t="s">
-        <v>55</v>
+        <v>46</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>12</v>
       </c>
       <c r="C17" s="8" t="s">
         <v>30</v>
@@ -1176,22 +1187,22 @@
       <c r="D17" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="E17" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="F17" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="G17" s="8" t="s">
-        <v>30</v>
+      <c r="E17" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="F17" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="G17" s="7" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="18" spans="1:7">
       <c r="A18" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>81</v>
+        <v>56</v>
+      </c>
+      <c r="B18" s="9" t="s">
+        <v>55</v>
       </c>
       <c r="C18" s="8" t="s">
         <v>30</v>
@@ -1205,28 +1216,28 @@
       <c r="F18" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="G18" s="7" t="s">
-        <v>29</v>
+      <c r="G18" s="8" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="19" spans="1:7">
       <c r="A19" s="1" t="s">
-        <v>47</v>
+        <v>82</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>22</v>
+        <v>81</v>
       </c>
       <c r="C19" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="D19" s="8" t="s">
-        <v>30</v>
+      <c r="D19" s="7" t="s">
+        <v>29</v>
       </c>
       <c r="E19" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="F19" s="7" t="s">
-        <v>29</v>
+      <c r="F19" s="8" t="s">
+        <v>30</v>
       </c>
       <c r="G19" s="7" t="s">
         <v>29</v>
@@ -1234,16 +1245,16 @@
     </row>
     <row r="20" spans="1:7">
       <c r="A20" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C20" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="D20" s="7" t="s">
-        <v>29</v>
+      <c r="D20" s="8" t="s">
+        <v>30</v>
       </c>
       <c r="E20" s="7" t="s">
         <v>29</v>
@@ -1251,16 +1262,16 @@
       <c r="F20" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="G20" s="8" t="s">
-        <v>30</v>
+      <c r="G20" s="7" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="21" spans="1:7">
       <c r="A21" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>50</v>
+        <v>23</v>
       </c>
       <c r="C21" s="8" t="s">
         <v>30</v>
@@ -1274,16 +1285,16 @@
       <c r="F21" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="G21" s="7" t="s">
-        <v>29</v>
+      <c r="G21" s="8" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="22" spans="1:7">
       <c r="A22" s="1" t="s">
-        <v>75</v>
+        <v>49</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>74</v>
+        <v>50</v>
       </c>
       <c r="C22" s="8" t="s">
         <v>30</v>
@@ -1291,22 +1302,22 @@
       <c r="D22" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="E22" s="8" t="s">
-        <v>30</v>
+      <c r="E22" s="7" t="s">
+        <v>29</v>
       </c>
       <c r="F22" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="G22" s="8" t="s">
-        <v>30</v>
+      <c r="G22" s="7" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="23" spans="1:7">
       <c r="A23" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>10</v>
+        <v>74</v>
       </c>
       <c r="C23" s="8" t="s">
         <v>30</v>
@@ -1317,19 +1328,19 @@
       <c r="E23" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="F23" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="G23" s="7" t="s">
-        <v>29</v>
+      <c r="F23" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="G23" s="8" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="24" spans="1:7">
       <c r="A24" s="1" t="s">
-        <v>51</v>
+        <v>76</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C24" s="8" t="s">
         <v>30</v>
@@ -1337,11 +1348,11 @@
       <c r="D24" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="E24" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="F24" s="7" t="s">
-        <v>29</v>
+      <c r="E24" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="F24" s="8" t="s">
+        <v>30</v>
       </c>
       <c r="G24" s="7" t="s">
         <v>29</v>
@@ -1349,10 +1360,10 @@
     </row>
     <row r="25" spans="1:7">
       <c r="A25" s="1" t="s">
-        <v>83</v>
+        <v>51</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>67</v>
+        <v>11</v>
       </c>
       <c r="C25" s="8" t="s">
         <v>30</v>
@@ -1363,8 +1374,8 @@
       <c r="E25" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="F25" s="8" t="s">
-        <v>30</v>
+      <c r="F25" s="7" t="s">
+        <v>29</v>
       </c>
       <c r="G25" s="7" t="s">
         <v>29</v>
@@ -1372,56 +1383,56 @@
     </row>
     <row r="26" spans="1:7">
       <c r="A26" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="C26" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="D26" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="E26" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="F26" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="G26" s="7" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7">
+      <c r="A27" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="B26" s="1" t="s">
+      <c r="B27" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="C26" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="D26" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="E26" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="F26" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="G26" s="7" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7">
-      <c r="A27" s="3" t="s">
+      <c r="C27" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="D27" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="E27" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="F27" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="G27" s="7" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7">
+      <c r="A28" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="B27" s="3" t="s">
+      <c r="B28" s="3" t="s">
         <v>69</v>
-      </c>
-      <c r="C27" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="D27" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="E27" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="F27" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="G27" s="7" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7">
-      <c r="A28" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="B28" s="1" t="s">
-        <v>27</v>
       </c>
       <c r="C28" s="8" t="s">
         <v>30</v>
@@ -1441,19 +1452,19 @@
     </row>
     <row r="29" spans="1:7">
       <c r="A29" s="1" t="s">
-        <v>73</v>
+        <v>57</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>5</v>
+        <v>27</v>
       </c>
       <c r="C29" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="D29" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="E29" s="7" t="s">
-        <v>29</v>
+      <c r="D29" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="E29" s="8" t="s">
+        <v>30</v>
       </c>
       <c r="F29" s="7" t="s">
         <v>29</v>
@@ -1464,10 +1475,10 @@
     </row>
     <row r="30" spans="1:7">
       <c r="A30" s="1" t="s">
-        <v>89</v>
+        <v>73</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>90</v>
+        <v>5</v>
       </c>
       <c r="C30" s="8" t="s">
         <v>30</v>
@@ -1478,19 +1489,19 @@
       <c r="E30" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="F30" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="G30" s="8" t="s">
-        <v>30</v>
+      <c r="F30" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="G30" s="7" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="31" spans="1:7">
       <c r="A31" s="1" t="s">
-        <v>58</v>
+        <v>89</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>3</v>
+        <v>90</v>
       </c>
       <c r="C31" s="8" t="s">
         <v>30</v>
@@ -1510,10 +1521,10 @@
     </row>
     <row r="32" spans="1:7">
       <c r="A32" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C32" s="8" t="s">
         <v>30</v>
@@ -1521,22 +1532,22 @@
       <c r="D32" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="E32" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="F32" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="G32" s="7" t="s">
-        <v>29</v>
+      <c r="E32" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="F32" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="G32" s="8" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="33" spans="1:7">
       <c r="A33" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C33" s="8" t="s">
         <v>30</v>
@@ -1547,117 +1558,117 @@
       <c r="E33" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="F33" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="G33" s="8" t="s">
-        <v>30</v>
+      <c r="F33" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="G33" s="7" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="34" spans="1:7">
       <c r="A34" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C34" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="D34" s="8" t="s">
-        <v>30</v>
+      <c r="D34" s="7" t="s">
+        <v>29</v>
       </c>
       <c r="E34" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="F34" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="G34" s="7" t="s">
-        <v>29</v>
+      <c r="F34" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="G34" s="8" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="35" spans="1:7">
       <c r="A35" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C35" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="D35" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="E35" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="F35" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="G35" s="7" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7">
+      <c r="A36" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="B35" s="1" t="s">
+      <c r="B36" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C35" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="D35" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="E35" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="F35" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="G35" s="8" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="36" spans="1:7">
-      <c r="A36" s="2" t="s">
+      <c r="C36" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="D36" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="E36" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="F36" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="G36" s="8" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7">
+      <c r="A37" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="B36" s="2" t="s">
+      <c r="B37" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="C36" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="D36" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="E36" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="F36" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="G36" s="8" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="37" spans="1:7">
-      <c r="A37" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="B37" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="C37" s="7" t="s">
-        <v>29</v>
+      <c r="C37" s="8" t="s">
+        <v>30</v>
       </c>
       <c r="D37" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="E37" s="8" t="s">
-        <v>30</v>
+      <c r="E37" s="7" t="s">
+        <v>29</v>
       </c>
       <c r="F37" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="G37" s="7" t="s">
-        <v>29</v>
+      <c r="G37" s="8" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="38" spans="1:7">
       <c r="A38" s="1" t="s">
-        <v>87</v>
+        <v>64</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="C38" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="D38" s="8" t="s">
-        <v>30</v>
+        <v>17</v>
+      </c>
+      <c r="C38" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="D38" s="7" t="s">
+        <v>29</v>
       </c>
       <c r="E38" s="8" t="s">
         <v>30</v>
@@ -1671,10 +1682,10 @@
     </row>
     <row r="39" spans="1:7">
       <c r="A39" s="1" t="s">
-        <v>65</v>
+        <v>87</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>21</v>
+        <v>86</v>
       </c>
       <c r="C39" s="8" t="s">
         <v>30</v>
@@ -1683,58 +1694,81 @@
         <v>30</v>
       </c>
       <c r="E39" s="8" t="s">
-        <v>31</v>
-      </c>
-      <c r="F39" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="G39" s="8" t="s">
-        <v>30</v>
+        <v>30</v>
+      </c>
+      <c r="F39" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="G39" s="7" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="40" spans="1:7">
       <c r="A40" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C40" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="D40" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="E40" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="F40" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="G40" s="8" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7">
+      <c r="A41" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="B40" s="1" t="s">
+      <c r="B41" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="C40" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="D40" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="E40" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="F40" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="G40" s="7" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="41" spans="1:7">
-      <c r="A41" s="3" t="s">
+      <c r="C41" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="D41" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="E41" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="F41" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="G41" s="7" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7">
+      <c r="A42" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="B41" s="3" t="s">
+      <c r="B42" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="C41" s="7" t="s">
+      <c r="C42" s="7" t="s">
         <v>91</v>
       </c>
-      <c r="D41" s="8">
-        <v>30</v>
-      </c>
-      <c r="E41" s="8">
-        <v>30</v>
-      </c>
-      <c r="F41" s="8">
-        <v>30</v>
-      </c>
-      <c r="G41" s="8" t="s">
+      <c r="D42" s="8">
+        <v>30</v>
+      </c>
+      <c r="E42" s="8">
+        <v>30</v>
+      </c>
+      <c r="F42" s="8">
+        <v>30</v>
+      </c>
+      <c r="G42" s="8" t="s">
         <v>77</v>
       </c>
     </row>
@@ -1745,7 +1779,7 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="0" r:id="rId1"/>
   <ignoredErrors>
-    <ignoredError sqref="G41" numberStoredAsText="1"/>
+    <ignoredError sqref="G42" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
fix compare last clips
</commit_message>
<xml_diff>
--- a/Publication/ClipboardManagerComparison.xlsx
+++ b/Publication/ClipboardManagerComparison.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="45" windowWidth="28755" windowHeight="12285"/>
+    <workbookView xWindow="0" yWindow="45" windowWidth="28755" windowHeight="12285" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="ааа" sheetId="1" r:id="rId1"/>
@@ -16,10 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="289" uniqueCount="97">
-  <si>
-    <t>Feature</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="297" uniqueCount="100">
   <si>
     <t>Paste in elevated window</t>
   </si>
@@ -164,9 +161,6 @@
     <t>-+</t>
   </si>
   <si>
-    <t>Возможность</t>
-  </si>
-  <si>
     <t>Сравнение клипов (команда)</t>
   </si>
   <si>
@@ -366,9 +360,6 @@
     <t>Paste in any input language and keyboard</t>
   </si>
   <si>
-    <t>70</t>
-  </si>
-  <si>
     <t>1.35</t>
   </si>
   <si>
@@ -382,6 +373,24 @@
   </si>
   <si>
     <t>5.23</t>
+  </si>
+  <si>
+    <t>Синхронизация буфера обмена между компьютерами</t>
+  </si>
+  <si>
+    <t>Sync clipboard between computers</t>
+  </si>
+  <si>
+    <t>Version</t>
+  </si>
+  <si>
+    <t>Clipboard manager</t>
+  </si>
+  <si>
+    <t>Менеджер буфера обмена</t>
+  </si>
+  <si>
+    <t>Версия</t>
   </si>
 </sst>
 </file>
@@ -481,7 +490,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -499,6 +508,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -796,10 +808,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G42"/>
+  <dimension ref="A1:G43"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:G1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -812,964 +824,991 @@
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1" s="4" t="s">
-        <v>32</v>
+        <v>98</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>0</v>
+        <v>97</v>
       </c>
       <c r="C1" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="E1" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="F1" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="F1" s="6" t="s">
-        <v>9</v>
-      </c>
       <c r="G1" s="6" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="2" spans="1:7">
-      <c r="A2" s="4"/>
-      <c r="B2" s="4"/>
+      <c r="A2" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>96</v>
+      </c>
       <c r="C2" s="6" t="s">
+        <v>89</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>93</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>90</v>
+      </c>
+      <c r="F2" s="6" t="s">
+        <v>91</v>
+      </c>
+      <c r="G2" s="6" t="s">
         <v>92</v>
-      </c>
-      <c r="D2" s="6" t="s">
-        <v>96</v>
-      </c>
-      <c r="E2" s="6" t="s">
-        <v>93</v>
-      </c>
-      <c r="F2" s="6" t="s">
-        <v>94</v>
-      </c>
-      <c r="G2" s="6" t="s">
-        <v>95</v>
       </c>
     </row>
     <row r="3" spans="1:7">
       <c r="A3" s="1" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E3" s="8" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F3" s="7" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G3" s="7" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="4" spans="1:7">
       <c r="A4" s="3" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E4" s="8" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F4" s="7" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G4" s="7" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="5" spans="1:7">
       <c r="A5" s="1" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C5" s="8" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D5" s="7" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E5" s="8" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F5" s="8" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G5" s="8" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="6" spans="1:7">
       <c r="A6" s="1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D6" s="8" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E6" s="8" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F6" s="7" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G6" s="7" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="7" spans="1:7">
       <c r="A7" s="1" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C7" s="8" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D7" s="7" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E7" s="7" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F7" s="8" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G7" s="8" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="8" spans="1:7">
       <c r="A8" s="1" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C8" s="8" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D8" s="7" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E8" s="7" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F8" s="8" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G8" s="8" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="9" spans="1:7">
       <c r="A9" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D9" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="E9" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="F9" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="E9" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="F9" s="8" t="s">
-        <v>31</v>
-      </c>
       <c r="G9" s="7" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="10" spans="1:7">
       <c r="A10" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D10" s="7" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E10" s="8" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F10" s="7" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G10" s="7" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="11" spans="1:7">
       <c r="A11" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C11" s="8" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D11" s="7" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E11" s="7" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F11" s="8" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G11" s="8" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="12" spans="1:7">
       <c r="A12" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C12" s="8" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D12" s="7" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E12" s="8" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F12" s="7" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G12" s="7" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="13" spans="1:7">
       <c r="A13" s="1" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C13" s="8" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D13" s="8" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E13" s="7" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F13" s="7" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G13" s="7" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="14" spans="1:7">
       <c r="A14" s="3" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C14" s="8" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D14" s="8" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E14" s="8" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F14" s="8" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G14" s="7" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="15" spans="1:7">
       <c r="A15" s="1" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C15" s="8" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D15" s="8" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E15" s="8" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F15" s="7" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G15" s="8" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="16" spans="1:7">
       <c r="A16" s="1" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C16" s="8" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D16" s="7" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E16" s="7" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F16" s="7" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G16" s="7" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="17" spans="1:7">
       <c r="A17" s="1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C17" s="8" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D17" s="7" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E17" s="8" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F17" s="7" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G17" s="7" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="18" spans="1:7">
       <c r="A18" s="1" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B18" s="9" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C18" s="8" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D18" s="7" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E18" s="7" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F18" s="8" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G18" s="8" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="19" spans="1:7">
       <c r="A19" s="1" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C19" s="8" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D19" s="7" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E19" s="7" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F19" s="8" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G19" s="7" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="20" spans="1:7">
       <c r="A20" s="1" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C20" s="8" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D20" s="8" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E20" s="7" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F20" s="7" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G20" s="7" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="21" spans="1:7">
       <c r="A21" s="1" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C21" s="8" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D21" s="7" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E21" s="7" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F21" s="7" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G21" s="8" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="22" spans="1:7">
       <c r="A22" s="1" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C22" s="8" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D22" s="7" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E22" s="7" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F22" s="7" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G22" s="7" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="23" spans="1:7">
       <c r="A23" s="1" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C23" s="8" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D23" s="7" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E23" s="8" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F23" s="7" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G23" s="8" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="24" spans="1:7">
       <c r="A24" s="1" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C24" s="8" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D24" s="7" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E24" s="8" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F24" s="8" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G24" s="7" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="25" spans="1:7">
       <c r="A25" s="1" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C25" s="8" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D25" s="7" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E25" s="7" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F25" s="7" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G25" s="7" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="26" spans="1:7">
       <c r="A26" s="1" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C26" s="8" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D26" s="7" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E26" s="7" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F26" s="8" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G26" s="7" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="27" spans="1:7">
       <c r="A27" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C27" s="8" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D27" s="8" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E27" s="8" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F27" s="7" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G27" s="7" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="28" spans="1:7">
       <c r="A28" s="3" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C28" s="8" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D28" s="8" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E28" s="8" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F28" s="7" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G28" s="7" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="29" spans="1:7">
       <c r="A29" s="1" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C29" s="8" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D29" s="8" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E29" s="8" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F29" s="7" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G29" s="7" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="30" spans="1:7">
       <c r="A30" s="1" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C30" s="8" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D30" s="7" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E30" s="7" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F30" s="7" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G30" s="7" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="31" spans="1:7">
       <c r="A31" s="1" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C31" s="8" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D31" s="7" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E31" s="7" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F31" s="8" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G31" s="8" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="32" spans="1:7">
       <c r="A32" s="1" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C32" s="8" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D32" s="7" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E32" s="7" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F32" s="8" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G32" s="8" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="33" spans="1:7">
       <c r="A33" s="1" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C33" s="8" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D33" s="7" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E33" s="8" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F33" s="7" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G33" s="7" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="34" spans="1:7">
       <c r="A34" s="1" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C34" s="8" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D34" s="7" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E34" s="8" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F34" s="8" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G34" s="8" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="35" spans="1:7">
       <c r="A35" s="1" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C35" s="8" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D35" s="8" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E35" s="8" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F35" s="7" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G35" s="7" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="36" spans="1:7">
       <c r="A36" s="1" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C36" s="8" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D36" s="7" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E36" s="8" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F36" s="7" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G36" s="8" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="37" spans="1:7">
       <c r="A37" s="2" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C37" s="8" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D37" s="7" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E37" s="7" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F37" s="7" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G37" s="8" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="38" spans="1:7">
       <c r="A38" s="1" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C38" s="7" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D38" s="7" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E38" s="8" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F38" s="7" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G38" s="7" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="39" spans="1:7">
       <c r="A39" s="1" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C39" s="8" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D39" s="8" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E39" s="8" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F39" s="7" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G39" s="7" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="40" spans="1:7">
       <c r="A40" s="1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C40" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="D40" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="E40" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="D40" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="E40" s="8" t="s">
-        <v>31</v>
-      </c>
       <c r="F40" s="8" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G40" s="8" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="41" spans="1:7">
       <c r="A41" s="1" t="s">
-        <v>66</v>
+        <v>94</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>88</v>
+        <v>95</v>
       </c>
       <c r="C41" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="D41" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="D41" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="E41" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="F41" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="G41" s="7" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7">
+      <c r="A42" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="C42" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="D42" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="E42" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="F42" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="G42" s="7" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7">
+      <c r="A43" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="B43" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C43" s="10">
+        <v>80</v>
+      </c>
+      <c r="D43" s="8">
         <v>30</v>
       </c>
-      <c r="E41" s="8" t="s">
+      <c r="E43" s="8">
         <v>30</v>
       </c>
-      <c r="F41" s="8" t="s">
+      <c r="F43" s="8">
         <v>30</v>
       </c>
-      <c r="G41" s="7" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="42" spans="1:7">
-      <c r="A42" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="B42" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="C42" s="7" t="s">
-        <v>91</v>
-      </c>
-      <c r="D42" s="8">
-        <v>30</v>
-      </c>
-      <c r="E42" s="8">
-        <v>30</v>
-      </c>
-      <c r="F42" s="8">
-        <v>30</v>
-      </c>
-      <c r="G42" s="8" t="s">
-        <v>77</v>
+      <c r="G43" s="8" t="s">
+        <v>75</v>
       </c>
     </row>
   </sheetData>
@@ -1779,18 +1818,24 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="0" r:id="rId1"/>
   <ignoredErrors>
-    <ignoredError sqref="G42" numberStoredAsText="1"/>
+    <ignoredError sqref="G43" numberStoredAsText="1"/>
+    <ignoredError sqref="C2:E2 G2" twoDigitTextYear="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="B1:F1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G4" sqref="A1:XFD1048576"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="2" max="6" width="9.140625" style="5"/>
+  </cols>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
+ monitor clipboard setting
</commit_message>
<xml_diff>
--- a/Publication/ClipboardManagerComparison.xlsx
+++ b/Publication/ClipboardManagerComparison.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="45" windowWidth="28755" windowHeight="12285" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="45" windowWidth="28755" windowHeight="12285"/>
   </bookViews>
   <sheets>
     <sheet name="ааа" sheetId="1" r:id="rId1"/>
@@ -810,8 +810,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G43"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:G1048576"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1249,8 +1249,8 @@
       <c r="D19" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="E19" s="7" t="s">
-        <v>28</v>
+      <c r="E19" s="8" t="s">
+        <v>29</v>
       </c>
       <c r="F19" s="8" t="s">
         <v>29</v>
@@ -1828,7 +1828,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B1:F1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G4" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
+ hotkey switch monitoring
</commit_message>
<xml_diff>
--- a/Publication/ClipboardManagerComparison.xlsx
+++ b/Publication/ClipboardManagerComparison.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="297" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="551" uniqueCount="100">
   <si>
     <t>Paste in elevated window</t>
   </si>
@@ -360,9 +360,6 @@
     <t>Paste in any input language and keyboard</t>
   </si>
   <si>
-    <t>1.35</t>
-  </si>
-  <si>
     <t>3.21</t>
   </si>
   <si>
@@ -391,6 +388,9 @@
   </si>
   <si>
     <t>Версия</t>
+  </si>
+  <si>
+    <t>1.40</t>
   </si>
 </sst>
 </file>
@@ -810,8 +810,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -824,10 +824,10 @@
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1" s="4" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C1" s="6" t="s">
         <v>5</v>
@@ -847,25 +847,25 @@
     </row>
     <row r="2" spans="1:7">
       <c r="A2" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="C2" s="6" t="s">
         <v>99</v>
       </c>
-      <c r="B2" s="4" t="s">
-        <v>96</v>
-      </c>
-      <c r="C2" s="6" t="s">
+      <c r="D2" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="E2" s="6" t="s">
         <v>89</v>
       </c>
-      <c r="D2" s="6" t="s">
-        <v>93</v>
-      </c>
-      <c r="E2" s="6" t="s">
+      <c r="F2" s="6" t="s">
         <v>90</v>
       </c>
-      <c r="F2" s="6" t="s">
+      <c r="G2" s="6" t="s">
         <v>91</v>
-      </c>
-      <c r="G2" s="6" t="s">
-        <v>92</v>
       </c>
     </row>
     <row r="3" spans="1:7">
@@ -1744,10 +1744,10 @@
     </row>
     <row r="41" spans="1:7">
       <c r="A41" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="B41" s="1" t="s">
         <v>94</v>
-      </c>
-      <c r="B41" s="1" t="s">
-        <v>95</v>
       </c>
       <c r="C41" s="7" t="s">
         <v>28</v>
@@ -1819,24 +1819,886 @@
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="0" r:id="rId1"/>
   <ignoredErrors>
     <ignoredError sqref="G43" numberStoredAsText="1"/>
-    <ignoredError sqref="C2:E2 G2" twoDigitTextYear="1"/>
+    <ignoredError sqref="D2:E2 G2" twoDigitTextYear="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B1:F1"/>
+  <dimension ref="A1:F43"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G4" sqref="A1:XFD1048576"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="6" width="9.140625" style="5"/>
+    <col min="1" max="1" width="59.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="5" width="9.140625" style="5"/>
   </cols>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:6">
+      <c r="A1" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="E1" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="F1" s="6" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>99</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>89</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>90</v>
+      </c>
+      <c r="F2" s="6" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="C3" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="D3" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="E3" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="F3" s="7" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="B4" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="D4" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="E4" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="F4" s="7" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B5" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="C5" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="D5" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="E5" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="F5" s="8" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="C6" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="D6" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="E6" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="F6" s="7" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="A7" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B7" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="C7" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="D7" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="E7" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="F7" s="8" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
+      <c r="A8" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B8" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="C8" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="D8" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="E8" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="F8" s="8" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
+      <c r="A9" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B9" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="C9" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="D9" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="E9" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="F9" s="7" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
+      <c r="A10" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B10" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="C10" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="D10" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="E10" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="F10" s="7" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
+      <c r="A11" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B11" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="C11" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="D11" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="E11" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="F11" s="8" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6">
+      <c r="A12" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B12" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="C12" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="D12" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="E12" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="F12" s="7" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6">
+      <c r="A13" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B13" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="C13" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="D13" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="E13" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="F13" s="7" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6">
+      <c r="A14" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="B14" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="C14" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="D14" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="E14" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="F14" s="7" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6">
+      <c r="A15" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B15" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="C15" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="D15" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="E15" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="F15" s="8" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6">
+      <c r="A16" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="B16" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="C16" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="D16" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="E16" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="F16" s="7" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6">
+      <c r="A17" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B17" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="C17" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="D17" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="E17" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="F17" s="7" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6">
+      <c r="A18" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B18" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="C18" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="D18" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="E18" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="F18" s="8" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6">
+      <c r="A19" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="B19" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="C19" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="D19" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="E19" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="F19" s="7" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6">
+      <c r="A20" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B20" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="C20" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="D20" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="E20" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="F20" s="7" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6">
+      <c r="A21" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B21" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="C21" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="D21" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="E21" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="F21" s="8" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6">
+      <c r="A22" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B22" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="C22" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="D22" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="E22" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="F22" s="7" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6">
+      <c r="A23" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="B23" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="C23" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="D23" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="E23" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="F23" s="8" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6">
+      <c r="A24" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="B24" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="C24" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="D24" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="E24" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="F24" s="7" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6">
+      <c r="A25" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B25" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="C25" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="D25" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="E25" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="F25" s="7" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6">
+      <c r="A26" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="B26" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="C26" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="D26" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="E26" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="F26" s="7" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6">
+      <c r="A27" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B27" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="C27" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="D27" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="E27" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="F27" s="7" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6">
+      <c r="A28" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="B28" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="C28" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="D28" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="E28" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="F28" s="7" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6">
+      <c r="A29" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B29" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="C29" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="D29" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="E29" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="F29" s="7" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6">
+      <c r="A30" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="B30" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="C30" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="D30" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="E30" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="F30" s="7" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6">
+      <c r="A31" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="B31" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="C31" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="D31" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="E31" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="F31" s="8" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6">
+      <c r="A32" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="B32" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="C32" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="D32" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="E32" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="F32" s="8" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6">
+      <c r="A33" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="B33" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="C33" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="D33" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="E33" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="F33" s="7" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6">
+      <c r="A34" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="B34" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="C34" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="D34" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="E34" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="F34" s="8" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6">
+      <c r="A35" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="B35" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="C35" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="D35" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="E35" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="F35" s="7" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6">
+      <c r="A36" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="B36" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="C36" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="D36" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="E36" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="F36" s="8" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6">
+      <c r="A37" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="B37" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="C37" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="D37" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="E37" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="F37" s="8" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6">
+      <c r="A38" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="B38" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="C38" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="D38" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="E38" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="F38" s="7" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6">
+      <c r="A39" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B39" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="C39" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="D39" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="E39" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="F39" s="7" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6">
+      <c r="A40" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B40" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="C40" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="D40" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="E40" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="F40" s="8" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6">
+      <c r="A41" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="B41" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="C41" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="D41" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="E41" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="F41" s="7" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6">
+      <c r="A42" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="B42" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="C42" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="D42" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="E42" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="F42" s="7" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6">
+      <c r="A43" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="B43" s="10">
+        <v>80</v>
+      </c>
+      <c r="C43" s="8">
+        <v>30</v>
+      </c>
+      <c r="D43" s="8">
+        <v>30</v>
+      </c>
+      <c r="E43" s="8">
+        <v>30</v>
+      </c>
+      <c r="F43" s="8" t="s">
+        <v>75</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
fix mark many filter words in HTML
</commit_message>
<xml_diff>
--- a/Publication/ClipboardManagerComparison.xlsx
+++ b/Publication/ClipboardManagerComparison.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="551" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="593" uniqueCount="103">
   <si>
     <t>Paste in elevated window</t>
   </si>
@@ -392,12 +392,21 @@
   <si>
     <t>1.40</t>
   </si>
+  <si>
+    <t>1.45</t>
+  </si>
+  <si>
+    <t>Clibor</t>
+  </si>
+  <si>
+    <t>1.4.9</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="4">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -431,6 +440,21 @@
       <charset val="204"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color indexed="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color indexed="17"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -450,7 +474,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -484,13 +508,28 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -510,6 +549,21 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="3" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="3" borderId="3" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -808,10 +862,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G43"/>
+  <dimension ref="A1:H43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H24" sqref="H24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -822,7 +876,7 @@
     <col min="4" max="7" width="8.7109375" style="5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:8">
       <c r="A1" s="4" t="s">
         <v>97</v>
       </c>
@@ -844,8 +898,11 @@
       <c r="G1" s="6" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="2" spans="1:7">
+      <c r="H1" s="11" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8">
       <c r="A2" s="4" t="s">
         <v>98</v>
       </c>
@@ -853,7 +910,7 @@
         <v>95</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="D2" s="6" t="s">
         <v>92</v>
@@ -867,8 +924,11 @@
       <c r="G2" s="6" t="s">
         <v>91</v>
       </c>
-    </row>
-    <row r="3" spans="1:7">
+      <c r="H2" s="12" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8">
       <c r="A3" s="1" t="s">
         <v>83</v>
       </c>
@@ -890,8 +950,11 @@
       <c r="G3" s="7" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="4" spans="1:7">
+      <c r="H3" s="13" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8">
       <c r="A4" s="3" t="s">
         <v>31</v>
       </c>
@@ -913,8 +976,11 @@
       <c r="G4" s="7" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="5" spans="1:7">
+      <c r="H4" s="14" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8">
       <c r="A5" s="1" t="s">
         <v>33</v>
       </c>
@@ -936,8 +1002,11 @@
       <c r="G5" s="8" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="6" spans="1:7">
+      <c r="H5" s="13" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8">
       <c r="A6" s="1" t="s">
         <v>34</v>
       </c>
@@ -959,8 +1028,11 @@
       <c r="G6" s="7" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="7" spans="1:7">
+      <c r="H6" s="13" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8">
       <c r="A7" s="1" t="s">
         <v>35</v>
       </c>
@@ -982,8 +1054,11 @@
       <c r="G7" s="8" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="8" spans="1:7">
+      <c r="H7" s="14" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8">
       <c r="A8" s="1" t="s">
         <v>51</v>
       </c>
@@ -1005,8 +1080,11 @@
       <c r="G8" s="8" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="9" spans="1:7">
+      <c r="H8" s="14" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8">
       <c r="A9" s="1" t="s">
         <v>36</v>
       </c>
@@ -1028,8 +1106,11 @@
       <c r="G9" s="7" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="10" spans="1:7">
+      <c r="H9" s="13" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8">
       <c r="A10" s="1" t="s">
         <v>37</v>
       </c>
@@ -1051,8 +1132,11 @@
       <c r="G10" s="7" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="11" spans="1:7">
+      <c r="H10" s="14" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8">
       <c r="A11" s="1" t="s">
         <v>38</v>
       </c>
@@ -1074,8 +1158,11 @@
       <c r="G11" s="8" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="12" spans="1:7">
+      <c r="H11" s="13" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8">
       <c r="A12" s="1" t="s">
         <v>40</v>
       </c>
@@ -1097,8 +1184,11 @@
       <c r="G12" s="7" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="13" spans="1:7">
+      <c r="H12" s="14" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8">
       <c r="A13" s="1" t="s">
         <v>41</v>
       </c>
@@ -1120,8 +1210,11 @@
       <c r="G13" s="7" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="14" spans="1:7">
+      <c r="H13" s="14" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8">
       <c r="A14" s="3" t="s">
         <v>70</v>
       </c>
@@ -1143,8 +1236,11 @@
       <c r="G14" s="7" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="15" spans="1:7">
+      <c r="H14" s="13" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8">
       <c r="A15" s="1" t="s">
         <v>43</v>
       </c>
@@ -1166,8 +1262,11 @@
       <c r="G15" s="8" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="16" spans="1:7">
+      <c r="H15" s="13" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8">
       <c r="A16" s="1" t="s">
         <v>78</v>
       </c>
@@ -1189,8 +1288,11 @@
       <c r="G16" s="7" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="17" spans="1:7">
+      <c r="H16" s="14" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8">
       <c r="A17" s="1" t="s">
         <v>44</v>
       </c>
@@ -1212,8 +1314,11 @@
       <c r="G17" s="7" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="18" spans="1:7">
+      <c r="H17" s="14" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8">
       <c r="A18" s="1" t="s">
         <v>54</v>
       </c>
@@ -1235,8 +1340,11 @@
       <c r="G18" s="8" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="19" spans="1:7">
+      <c r="H18" s="14" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8">
       <c r="A19" s="1" t="s">
         <v>80</v>
       </c>
@@ -1258,8 +1366,11 @@
       <c r="G19" s="7" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="20" spans="1:7">
+      <c r="H19" s="14" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8">
       <c r="A20" s="1" t="s">
         <v>45</v>
       </c>
@@ -1281,8 +1392,11 @@
       <c r="G20" s="7" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="21" spans="1:7">
+      <c r="H20" s="13" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8">
       <c r="A21" s="1" t="s">
         <v>46</v>
       </c>
@@ -1304,8 +1418,11 @@
       <c r="G21" s="8" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="22" spans="1:7">
+      <c r="H21" s="14" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8">
       <c r="A22" s="1" t="s">
         <v>47</v>
       </c>
@@ -1327,8 +1444,11 @@
       <c r="G22" s="7" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="23" spans="1:7">
+      <c r="H22" s="14" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8">
       <c r="A23" s="1" t="s">
         <v>73</v>
       </c>
@@ -1350,8 +1470,11 @@
       <c r="G23" s="8" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="24" spans="1:7">
+      <c r="H23" s="13" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8">
       <c r="A24" s="1" t="s">
         <v>74</v>
       </c>
@@ -1373,8 +1496,11 @@
       <c r="G24" s="7" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="25" spans="1:7">
+      <c r="H24" s="13" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8">
       <c r="A25" s="1" t="s">
         <v>49</v>
       </c>
@@ -1396,8 +1522,11 @@
       <c r="G25" s="7" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="26" spans="1:7">
+      <c r="H25" s="14" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8">
       <c r="A26" s="1" t="s">
         <v>81</v>
       </c>
@@ -1419,8 +1548,11 @@
       <c r="G26" s="7" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="27" spans="1:7">
+      <c r="H26" s="14" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8">
       <c r="A27" s="1" t="s">
         <v>50</v>
       </c>
@@ -1442,8 +1574,11 @@
       <c r="G27" s="7" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="28" spans="1:7">
+      <c r="H27" s="14" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8">
       <c r="A28" s="3" t="s">
         <v>66</v>
       </c>
@@ -1465,8 +1600,11 @@
       <c r="G28" s="7" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="29" spans="1:7">
+      <c r="H28" s="14" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8">
       <c r="A29" s="1" t="s">
         <v>55</v>
       </c>
@@ -1488,8 +1626,11 @@
       <c r="G29" s="7" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="30" spans="1:7">
+      <c r="H29" s="13" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8">
       <c r="A30" s="1" t="s">
         <v>71</v>
       </c>
@@ -1511,8 +1652,11 @@
       <c r="G30" s="7" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="31" spans="1:7">
+      <c r="H30" s="14" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8">
       <c r="A31" s="1" t="s">
         <v>87</v>
       </c>
@@ -1534,8 +1678,11 @@
       <c r="G31" s="8" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="32" spans="1:7">
+      <c r="H31" s="14" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8">
       <c r="A32" s="1" t="s">
         <v>56</v>
       </c>
@@ -1557,8 +1704,11 @@
       <c r="G32" s="8" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="33" spans="1:7">
+      <c r="H32" s="14" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8">
       <c r="A33" s="1" t="s">
         <v>57</v>
       </c>
@@ -1580,8 +1730,11 @@
       <c r="G33" s="7" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="34" spans="1:7">
+      <c r="H33" s="14" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8">
       <c r="A34" s="1" t="s">
         <v>58</v>
       </c>
@@ -1603,8 +1756,11 @@
       <c r="G34" s="8" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="35" spans="1:7">
+      <c r="H34" s="14" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8">
       <c r="A35" s="1" t="s">
         <v>59</v>
       </c>
@@ -1626,8 +1782,11 @@
       <c r="G35" s="7" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="36" spans="1:7">
+      <c r="H35" s="14" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8">
       <c r="A36" s="1" t="s">
         <v>60</v>
       </c>
@@ -1649,8 +1808,11 @@
       <c r="G36" s="8" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="37" spans="1:7">
+      <c r="H36" s="13" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8">
       <c r="A37" s="2" t="s">
         <v>61</v>
       </c>
@@ -1672,8 +1834,11 @@
       <c r="G37" s="8" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="38" spans="1:7">
+      <c r="H37" s="14" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8">
       <c r="A38" s="1" t="s">
         <v>62</v>
       </c>
@@ -1695,8 +1860,11 @@
       <c r="G38" s="7" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="39" spans="1:7">
+      <c r="H38" s="14" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8">
       <c r="A39" s="1" t="s">
         <v>85</v>
       </c>
@@ -1718,8 +1886,11 @@
       <c r="G39" s="7" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="40" spans="1:7">
+      <c r="H39" s="14" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8">
       <c r="A40" s="1" t="s">
         <v>63</v>
       </c>
@@ -1741,8 +1912,11 @@
       <c r="G40" s="8" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="41" spans="1:7">
+      <c r="H40" s="13" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8">
       <c r="A41" s="1" t="s">
         <v>93</v>
       </c>
@@ -1764,8 +1938,11 @@
       <c r="G41" s="7" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="42" spans="1:7">
+      <c r="H41" s="14" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8">
       <c r="A42" s="1" t="s">
         <v>64</v>
       </c>
@@ -1787,8 +1964,11 @@
       <c r="G42" s="7" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="43" spans="1:7">
+      <c r="H42" s="14" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8">
       <c r="A43" s="3" t="s">
         <v>68</v>
       </c>
@@ -1809,6 +1989,9 @@
       </c>
       <c r="G43" s="8" t="s">
         <v>75</v>
+      </c>
+      <c r="H43" s="15">
+        <v>20</v>
       </c>
     </row>
   </sheetData>
@@ -1819,7 +2002,7 @@
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="0" r:id="rId1"/>
   <ignoredErrors>
     <ignoredError sqref="G43" numberStoredAsText="1"/>
-    <ignoredError sqref="D2:E2 G2" twoDigitTextYear="1"/>
+    <ignoredError sqref="C2:E2 G2:H2" twoDigitTextYear="1"/>
   </ignoredErrors>
 </worksheet>
 </file>

</xml_diff>